<commit_message>
After Question 6 w/ Barchart
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Desktop\NSS DA11\Excel\lookups-exercise-DoubleM85\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076E5B23-48A6-40DB-83E1-8DB59B4CA70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFAA254-3C4B-4925-9900-68AAA8365C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -879,6 +879,983 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Budget vs Actual</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>356640100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382685200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376548600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-875A-417A-A6CF-566D179B7C13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>341243679.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>346340810.81999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>355279492.22999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-875A-417A-A6CF-566D179B7C13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1150628304"/>
+        <c:axId val="1151465728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1150628304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1151465728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1151465728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1150628304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69BF2521-FAEA-A877-69C8-B484B5DCBA16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1178,8 +2155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4814,16 +5791,14 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{DF9F61D9-5896-45C8-9530-BE0C2033D6BD}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
After Review - Refined #7 and revived #3
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Desktop\NSS DA11\Excel\lookups-exercise-DoubleM85\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BCDA5B-13FC-4251-B09E-3840253DA598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002CB165-F1F7-4C5E-8075-498806991097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +326,15 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 7.4</t>
+  </si>
+  <si>
+    <t>Question 7.3</t>
+  </si>
+  <si>
+    <t>Question 7.5</t>
   </si>
 </sst>
 </file>
@@ -1003,13 +1034,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>356640100</c:v>
+                  <c:v>5999400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>382685200</c:v>
+                  <c:v>6195500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>376548600</c:v>
+                  <c:v>6157400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,13 +1099,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>341243679.13</c:v>
+                  <c:v>5925637.7199999904</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>346340810.81999999</c:v>
+                  <c:v>6084985.4699999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>355279492.22999901</c:v>
+                  <c:v>5987572.0199999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1819,16 +1850,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1543050</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2155,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2195,7 @@
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.85546875" customWidth="1"/>
@@ -5236,6 +5267,9 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -5250,20 +5284,47 @@
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>24</v>
       </c>
       <c r="B56">
-        <f>INDEX($A$1:$P$52,MATCH($A56,$A$1:$A$52,0),MATCH(B$55,$A$1:$P$1,0))</f>
+        <f>VLOOKUP(A56,A$2:D$52,4,0)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:D56" si="9">INDEX($A$1:$P$52,MATCH($A56,$A$1:$A$52,0),MATCH(C$55,$A$1:$P$1,0))</f>
+        <f>VLOOKUP(A56,A2:I52,9,0)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
+        <f>VLOOKUP(A56,A2:N52,14,0)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <f>VLOOKUP($F56,$A$1:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:I56" si="9">VLOOKUP($F56,$A$1:$P$52,MATCH(H$55,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I56">
         <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
@@ -5273,15 +5334,30 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:D61" si="10">INDEX($A$1:$P$52,MATCH($A57,$A$1:$A$52,0),MATCH(B$55,$A$1:$P$1,0))</f>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP(A57,A$2:D$52,4,0)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="C57:C61" si="11">VLOOKUP(A57,A3:I53,9,0)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D57:D61" si="12">VLOOKUP(A57,A3:N53,14,0)</f>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:I61" si="13">VLOOKUP($F57,$A$1:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="13"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5294,11 +5370,26 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="13"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="13"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5311,11 +5402,26 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="13"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="13"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5328,11 +5434,26 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="13"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5345,11 +5466,26 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="13"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5357,6 +5493,9 @@
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="F63" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -5371,8 +5510,20 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5388,98 +5539,191 @@
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" cm="1">
+        <f t="array" ref="G65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H65" cm="1">
+        <f t="array" ref="H65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I65" cm="1">
+        <f t="array" ref="I65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="11">_xlfn.XLOOKUP(A66,A$2:A$52,D$2:D$52)</f>
+        <f t="shared" ref="B66:B70" si="14">_xlfn.XLOOKUP(A66,A$2:A$52,D$2:D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="12">_xlfn.XLOOKUP(A66,A$2:A$52,I$2:I$52)</f>
+        <f t="shared" ref="C66:C70" si="15">_xlfn.XLOOKUP(A66,A$2:A$52,I$2:I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" cm="1">
+        <f t="array" ref="G66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H66" cm="1">
+        <f t="array" ref="H66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I66" cm="1">
+        <f t="array" ref="I66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" cm="1">
+        <f t="array" ref="G67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H67" cm="1">
+        <f t="array" ref="H67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I67" cm="1">
+        <f t="array" ref="I67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68" cm="1">
+        <f t="array" ref="G68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H68" cm="1">
+        <f t="array" ref="H68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I68" cm="1">
+        <f t="array" ref="I68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" cm="1">
+        <f t="array" ref="G69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H69" cm="1">
+        <f t="array" ref="H69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I69" cm="1">
+        <f t="array" ref="I69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" cm="1">
+        <f t="array" ref="G70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H70" cm="1">
+        <f t="array" ref="H70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I70" cm="1">
+        <f t="array" ref="I70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$64,$A$1:$P$1,0)),FALSE)</f>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F72" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5492,8 +5736,20 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5509,89 +5765,179 @@
         <f>INDEX($N$1:$N$52,MATCH(A74,$A$1:$A$52))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74">
+        <f>INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H74">
+        <f t="shared" ref="H74:I74" si="17">INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(H$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="17"/>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="14">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52))</f>
+        <f t="shared" ref="B75:B79" si="18">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="15">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52))</f>
+        <f t="shared" ref="C75:C79" si="19">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="16">INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52))</f>
+        <f t="shared" ref="D75:D79" si="20">INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ref="G75:I79" si="21">INDEX($A$1:$P$52,MATCH($F75,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="21"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="21"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="21"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="21"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="21"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="21"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="21"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="21"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="21"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="21"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="21"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="21"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="21"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5619,11 +5965,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B$2:B$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>356640100</v>
+        <v>5999400</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C$2:C$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>341243679.13</v>
+        <v>5925637.7199999904</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -5632,11 +5978,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G$2:G$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>382685200</v>
+        <v>6195500</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H$2:H$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>346340810.81999999</v>
+        <v>6084985.4699999997</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -5645,16 +5991,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L$2:L$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>376548600</v>
+        <v>6157400</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M$2:M$52,MATCH($B$87,$A$2:$A$52))</f>
-        <v>355279492.22999901</v>
+        <v>5987572.0199999996</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>